<commit_message>
Changes to prepare for 2.10.0 merge. Mostly with ActivityHistory
</commit_message>
<xml_diff>
--- a/Database/UCSF/GadgetOrderSQLGenerator.xlsx
+++ b/Database/UCSF/GadgetOrderSQLGenerator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22035" windowHeight="10545"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22035" windowHeight="10545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Page" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>Faculty Mentoring</t>
   </si>
   <si>
-    <t>PopulationHealthSciences</t>
-  </si>
-  <si>
     <t>Student Projects</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Featured Videos</t>
+  </si>
+  <si>
+    <t>Population Health Sciences</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,16 +615,16 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE [Profile.Data].[Person.Filter] set PersonFilterSort = 4 WHERE PersonFilter = 'PopulationHealthSciences';</v>
+        <v>UPDATE [Profile.Data].[Person.Filter] set PersonFilterSort = 4 WHERE PersonFilter = 'Population Health Sciences';</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
@@ -633,7 +633,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
@@ -642,7 +642,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
@@ -651,7 +651,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
@@ -660,7 +660,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
@@ -669,7 +669,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -678,7 +678,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>

</xml_diff>